<commit_message>
Ajuste na planilha de Apoio
</commit_message>
<xml_diff>
--- a/Gestão/Status Report/Apoio 15-10-2015.xlsx
+++ b/Gestão/Status Report/Apoio 15-10-2015.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Previsto</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Qui 15/10/15</t>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -665,11 +668,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121230928"/>
-        <c:axId val="-2121227456"/>
+        <c:axId val="-2121608688"/>
+        <c:axId val="-2141456000"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2121230928"/>
+        <c:axId val="-2121608688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,14 +715,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121227456"/>
+        <c:crossAx val="-2141456000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2121227456"/>
+        <c:axId val="-2141456000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +773,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121230928"/>
+        <c:crossAx val="-2121608688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1754,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1884,6 +1887,11 @@
     <row r="5" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.2">

</xml_diff>